<commit_message>
Fixing test data, debugging and renamed "Sub Systems" to "Sub-Systems" throughout.
</commit_message>
<xml_diff>
--- a/dds/operations.xlsx
+++ b/dds/operations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8080" tabRatio="390" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8080" tabRatio="390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="369">
   <si>
     <t>Identifier</t>
   </si>
@@ -965,9 +965,6 @@
     <t>Requirements data for accessing device sub-systems</t>
   </si>
   <si>
-    <t>device.subsytem_maintenance</t>
-  </si>
-  <si>
     <t>device.subsystem_maintenance</t>
   </si>
   <si>
@@ -1113,9 +1110,6 @@
   </si>
   <si>
     <t>device.control_subsystem_failure_rates</t>
-  </si>
-  <si>
-    <t>device.subsystem_operations_weighting</t>
   </si>
   <si>
     <t>filter.view_sub_systems_operation_weightings</t>
@@ -1152,13 +1146,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1306,25 +1307,25 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1332,21 +1333,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -1775,10 +1777,10 @@
     </row>
     <row r="2" spans="1:8" s="17" customFormat="1">
       <c r="A2" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>308</v>
@@ -1789,26 +1791,26 @@
     </row>
     <row r="3" spans="1:8" s="17" customFormat="1">
       <c r="A3" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>322</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>323</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:8" s="17" customFormat="1">
       <c r="A4" s="21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>181</v>
@@ -1821,10 +1823,10 @@
     </row>
     <row r="5" spans="1:8" s="17" customFormat="1">
       <c r="A5" s="21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>121</v>
@@ -1835,10 +1837,10 @@
     </row>
     <row r="6" spans="1:8" s="17" customFormat="1" ht="14" customHeight="1">
       <c r="A6" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>104</v>
@@ -1849,10 +1851,10 @@
     </row>
     <row r="7" spans="1:8" s="17" customFormat="1">
       <c r="A7" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>76</v>
@@ -1863,24 +1865,24 @@
     </row>
     <row r="8" spans="1:8" s="17" customFormat="1">
       <c r="A8" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>350</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="17" customFormat="1">
       <c r="A9" s="21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>110</v>
@@ -1894,7 +1896,7 @@
         <v>307</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>308</v>
@@ -1908,13 +1910,13 @@
         <v>186</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>322</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>323</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
@@ -1924,7 +1926,7 @@
         <v>187</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>181</v>
@@ -1936,11 +1938,11 @@
       <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:8" s="17" customFormat="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="23" t="s">
         <v>306</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>121</v>
@@ -1951,10 +1953,10 @@
     </row>
     <row r="14" spans="1:8" s="17" customFormat="1" ht="14" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>104</v>
@@ -1964,11 +1966,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1">
-      <c r="A15" s="17" t="s">
-        <v>312</v>
+      <c r="A15" s="23" t="s">
+        <v>311</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>76</v>
@@ -1978,25 +1980,25 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="17" customFormat="1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>351</v>
-      </c>
     </row>
     <row r="17" spans="1:8" s="17" customFormat="1">
-      <c r="A17" s="17" t="s">
-        <v>313</v>
+      <c r="A17" s="23" t="s">
+        <v>312</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>110</v>
@@ -8077,7 +8079,7 @@
         <v>298</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>38</v>
@@ -9120,8 +9122,8 @@
   </sheetPr>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -9168,7 +9170,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
         <v>200</v>
@@ -9197,7 +9199,7 @@
     </row>
     <row r="3" spans="1:18" s="7" customFormat="1">
       <c r="A3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s">
         <v>200</v>
@@ -9239,7 +9241,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" t="s">
         <v>200</v>
@@ -9280,7 +9282,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B5" t="s">
         <v>200</v>
@@ -9300,21 +9302,24 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>352</v>
-      </c>
-      <c r="B6" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B7" t="s">
         <v>200</v>
@@ -9424,7 +9429,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B10" t="s">
         <v>200</v>
@@ -9465,7 +9470,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B11" t="s">
         <v>200</v>
@@ -9485,21 +9490,24 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="B12" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B13" t="s">
         <v>200</v>
@@ -10076,7 +10084,7 @@
   <dimension ref="A1:Z80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -10125,7 +10133,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
         <v>158</v>
@@ -10154,7 +10162,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>158</v>
@@ -10174,7 +10182,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
         <v>158</v>
@@ -10215,7 +10223,7 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>16</v>
@@ -10226,7 +10234,7 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>16</v>
@@ -10237,7 +10245,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>158</v>
@@ -10272,7 +10280,7 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>16</v>
@@ -10287,7 +10295,7 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
         <v>158</v>
@@ -10419,7 +10427,7 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" t="s">
         <v>158</v>
@@ -10460,7 +10468,7 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>158</v>
@@ -10480,7 +10488,7 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="11" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>16</v>
@@ -10495,7 +10503,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B17" t="s">
         <v>158</v>
@@ -11767,7 +11775,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B6" t="s">
         <v>101</v>
@@ -11808,7 +11816,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B7" t="s">
         <v>101</v>
@@ -11828,7 +11836,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B8" t="s">
         <v>101</v>
@@ -11869,7 +11877,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s">
         <v>101</v>
@@ -11898,7 +11906,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>73</v>
@@ -11909,7 +11917,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>171</v>
@@ -11920,7 +11928,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>101</v>
@@ -11955,7 +11963,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B13" t="s">
         <v>101</v>
@@ -11996,7 +12004,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B14" t="s">
         <v>101</v>
@@ -12016,7 +12024,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B15" t="s">
         <v>101</v>
@@ -12816,239 +12824,239 @@
         <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>333</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" t="s">
         <v>314</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>315</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>316</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H2" t="s">
         <v>317</v>
-      </c>
-      <c r="G2" t="s">
-        <v>319</v>
-      </c>
-      <c r="H2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>317</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>317</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>337</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>364</v>
       </c>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>315</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>326</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -13056,25 +13064,25 @@
         <v>307</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D10" t="s">
         <v>314</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>315</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>316</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
+        <v>318</v>
+      </c>
+      <c r="H10" t="s">
         <v>317</v>
-      </c>
-      <c r="G10" t="s">
-        <v>319</v>
-      </c>
-      <c r="H10" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -13082,13 +13090,13 @@
         <v>186</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>344</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>345</v>
       </c>
       <c r="E11" s="11"/>
     </row>
@@ -13097,13 +13105,13 @@
         <v>187</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E12" s="11"/>
     </row>
@@ -13112,157 +13120,157 @@
         <v>306</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="I13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>317</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="K14" s="10" t="s">
+      <c r="L14" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="M14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>317</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>337</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>364</v>
       </c>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>315</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G17" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="10" t="s">
         <v>326</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -13414,8 +13422,8 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -13443,7 +13451,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -13451,7 +13459,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
@@ -13459,7 +13467,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
@@ -13467,7 +13475,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
@@ -13475,7 +13483,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
@@ -13483,7 +13491,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
@@ -13491,7 +13499,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
@@ -13499,7 +13507,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
@@ -13564,7 +13572,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
@@ -13578,7 +13586,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B15" t="s">
         <v>57</v>
@@ -13593,7 +13601,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>

</xml_diff>